<commit_message>
Calculador de la cantidad de veces que se envía información
</commit_message>
<xml_diff>
--- a/Tablas_del_Tp3.xlsx
+++ b/Tablas_del_Tp3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seba-\Documents\mi_carpeta\UNIVERSIDAD\Finales\TP3_IDL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A97CD89F-78A0-4C65-9B77-D859393040CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F16FE5-0A2C-4013-A4B7-78EB0ACBD1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E0F4AA8-2183-4C1F-A931-EBB40DCEB182}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>Estado Actual</t>
   </si>
@@ -126,6 +126,42 @@
   </si>
   <si>
     <t>Q2\Q1\Q0 + \Q2Q1Q0</t>
+  </si>
+  <si>
+    <t>Columna5</t>
+  </si>
+  <si>
+    <t>Columna6</t>
+  </si>
+  <si>
+    <t>Columna7</t>
+  </si>
+  <si>
+    <t>Columna8</t>
+  </si>
+  <si>
+    <t>Columna9</t>
+  </si>
+  <si>
+    <t>Estados</t>
+  </si>
+  <si>
+    <t>LOAD</t>
+  </si>
+  <si>
+    <t>Estado 4</t>
+  </si>
+  <si>
+    <t>Estado 5</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -167,9 +203,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,6 +447,24 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{CFE5171F-FDB2-46DC-846B-2E95FAE50F1B}" name="Q futuros"/>
     <tableColumn id="2" xr3:uid="{79BE50E9-7757-4323-A7E8-921A78F46823}" name="Formulas"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E019A1BE-4372-4E77-A419-5135BC9C35AC}" name="Tabla7" displayName="Tabla7" ref="A31:I36" totalsRowShown="0">
+  <autoFilter ref="A31:I36" xr:uid="{E019A1BE-4372-4E77-A419-5135BC9C35AC}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{CA20093C-257C-4626-BF8C-B2633F472E7B}" name="Estados"/>
+    <tableColumn id="2" xr3:uid="{C9A62C25-C95C-4EF0-BD1D-0C02841113FA}" name="LOAD"/>
+    <tableColumn id="3" xr3:uid="{1DA1E9A3-2ECD-4B09-9399-EA9C41E59533}" name="STOP"/>
+    <tableColumn id="4" xr3:uid="{95E57412-E3C1-4A07-8CDD-62DAA57B9536}" name="DIRECCIÓN"/>
+    <tableColumn id="5" xr3:uid="{7849CEB5-0036-44C7-9E2D-E44B3FAD0FF3}" name="Columna5"/>
+    <tableColumn id="6" xr3:uid="{E54701C9-A103-4E6E-9044-04B386FB5555}" name="Columna6"/>
+    <tableColumn id="7" xr3:uid="{7D60CB72-26DE-4C79-889E-FDA905DEF687}" name="Columna7"/>
+    <tableColumn id="8" xr3:uid="{90CEE447-0AE0-4F18-894B-B12F1C98A9EF}" name="Columna8"/>
+    <tableColumn id="9" xr3:uid="{E09101C1-B896-4091-906C-B7BF79B74DDE}" name="Columna9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -734,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700EAF10-5D51-4EB3-80B9-A9651B947D36}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,7 +806,7 @@
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -776,7 +829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -799,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -822,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -845,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -868,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -897,7 +950,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -926,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -955,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -984,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1013,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1035,9 +1088,8 @@
       <c r="H15" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1060,7 +1112,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1083,7 +1135,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
         <v>26</v>
       </c>
@@ -1091,7 +1143,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1108,7 +1160,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1125,7 +1177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1142,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1159,7 +1211,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1176,7 +1228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1191,6 +1243,105 @@
       </c>
       <c r="E27">
         <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1198,13 +1349,14 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="6">
+  <tableParts count="7">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>